<commit_message>
Updated cumulativeLayoutShift to remove typo
</commit_message>
<xml_diff>
--- a/src/content/docs/oma/value-drivers/customer-experience/use-cases/quality-foundation/CustomerExperience_QualityFoundation_KPI.xlsx
+++ b/src/content/docs/oma/value-drivers/customer-experience/use-cases/quality-foundation/CustomerExperience_QualityFoundation_KPI.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
   <si>
     <t>KPI</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>CLS</t>
-  </si>
-  <si>
-    <t>0.1s</t>
   </si>
   <si>
     <t>LCP</t>
@@ -497,37 +494,37 @@
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>17</v>
+      <c r="B4" s="6">
+        <v>0.1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="7">
         <v>0.98</v>
@@ -535,26 +532,26 @@
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -621,7 +618,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
@@ -637,8 +634,8 @@
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>17</v>
+      <c r="B4" s="6">
+        <v>0.1</v>
       </c>
       <c r="C4" s="9">
         <v>0.00156</v>
@@ -646,10 +643,10 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="C5" s="9">
         <v>2.094</v>
@@ -657,10 +654,10 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="C6" s="9">
         <v>3.031</v>
@@ -668,10 +665,10 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="9">
         <v>1.078</v>
@@ -679,7 +676,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="10">
         <v>0.98</v>
@@ -690,10 +687,10 @@
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>25</v>
       </c>
       <c r="C9" s="11">
         <v>0.09</v>
@@ -701,10 +698,10 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="11">
         <v>0.1</v>
@@ -712,10 +709,10 @@
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="11">
         <v>0.13</v>
@@ -726,7 +723,7 @@
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="13"/>
     </row>
@@ -743,8 +740,8 @@
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>17</v>
+      <c r="B15" s="6">
+        <v>0.1</v>
       </c>
       <c r="C15" s="9">
         <v>0.176</v>
@@ -752,10 +749,10 @@
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="C16" s="14">
         <v>2.969</v>
@@ -763,10 +760,10 @@
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="C17" s="9">
         <v>59.0</v>
@@ -774,10 +771,10 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="14">
         <v>2.011</v>
@@ -785,7 +782,7 @@
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="7">
         <v>0.98</v>
@@ -796,10 +793,10 @@
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>25</v>
       </c>
       <c r="C20" s="15">
         <v>0.01</v>
@@ -807,10 +804,10 @@
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="11">
         <v>9.0E-4</v>
@@ -818,10 +815,10 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="11">
         <v>0.13</v>

</xml_diff>

<commit_message>
Updated Quality Foundation KPIs
</commit_message>
<xml_diff>
--- a/src/content/docs/oma/value-drivers/customer-experience/use-cases/quality-foundation/CustomerExperience_QualityFoundation_KPI.xlsx
+++ b/src/content/docs/oma/value-drivers/customer-experience/use-cases/quality-foundation/CustomerExperience_QualityFoundation_KPI.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="32">
   <si>
     <t>KPI</t>
   </si>
@@ -62,6 +62,12 @@
     <t>PageViews</t>
   </si>
   <si>
+    <t>TTFB</t>
+  </si>
+  <si>
+    <t>0.5 s</t>
+  </si>
+  <si>
     <t>CLS</t>
   </si>
   <si>
@@ -98,7 +104,10 @@
     <t>All countries, all devices</t>
   </si>
   <si>
-    <t>All countries, Mobile</t>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>All countries, Mobile Web</t>
   </si>
 </sst>
 </file>
@@ -182,34 +191,34 @@
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="9" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="4" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -491,26 +500,26 @@
       <c r="B3" s="5"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="6">
-        <v>0.1</v>
+      <c r="B4" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="6" t="s">
         <v>18</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0.1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -518,40 +527,48 @@
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>18</v>
+      <c r="B7" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="7">
-        <v>0.98</v>
+        <v>23</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="6" t="s">
         <v>24</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0.98</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>24</v>
+      <c r="B10" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>24</v>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -617,210 +634,232 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
-        <v>27</v>
+      <c r="A2" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="9">
         <v>365000.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0.00156</v>
+      <c r="A4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="11">
+        <v>1.9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="B5" s="7">
+        <v>0.1</v>
+      </c>
       <c r="C5" s="9">
-        <v>2.094</v>
+        <v>0.00156</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="9">
-        <v>3.031</v>
+        <v>2.094</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>18</v>
+      <c r="B7" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C7" s="9">
-        <v>1.078</v>
+        <v>3.031</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="10">
-        <v>0.98</v>
-      </c>
-      <c r="C8" s="11">
-        <v>0.81</v>
+        <v>23</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1.078</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="11">
-        <v>0.09</v>
+      <c r="B9" s="12">
+        <v>0.98</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0.81</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="11">
-        <v>0.1</v>
+      <c r="B10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0.09</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="11">
+      <c r="C11" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="13">
         <v>0.13</v>
       </c>
     </row>
-    <row r="12">
-      <c r="B12" s="13"/>
-    </row>
     <row r="13">
-      <c r="A13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="14"/>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="9">
-        <v>1460.0</v>
-      </c>
+      <c r="A14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="14"/>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="6">
-        <v>0.1</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B15" s="7"/>
       <c r="C15" s="9">
-        <v>0.176</v>
+        <v>1460.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="14">
-        <v>2.969</v>
+      <c r="C16" s="11">
+        <v>2.2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0.1</v>
       </c>
       <c r="C17" s="9">
-        <v>59.0</v>
+        <v>0.176</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="14">
-        <v>2.011</v>
+        <v>19</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="15">
+        <v>2.969</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="7">
-        <v>0.98</v>
-      </c>
       <c r="C19" s="9">
-        <v>99.0</v>
+        <v>59.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>24</v>
+      <c r="B20" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="C20" s="15">
-        <v>0.01</v>
+        <v>2.011</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="11">
-        <v>9.0E-4</v>
+      <c r="B21" s="8">
+        <v>0.98</v>
+      </c>
+      <c r="C21" s="9">
+        <v>99.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>24</v>
-      </c>
       <c r="C22" s="11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="13">
+        <v>9.0E-4</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="13">
         <v>0.13</v>
       </c>
     </row>

</xml_diff>